<commit_message>
add geography level column
</commit_message>
<xml_diff>
--- a/area_level_predictor_pairs.xlsx
+++ b/area_level_predictor_pairs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Desktop\leadmap-public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasse/Library/Mobile Documents/com~apple~CloudDocs/Oxford MPhil/GRA Frank/lead_map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA658815-719C-4448-BED0-A0EC212F4DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1424A1EC-13CA-DC48-958F-02D0418B4BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="area_level_matches" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="947">
   <si>
     <t>variable</t>
   </si>
@@ -3091,6 +3091,21 @@
   </si>
   <si>
     <t xml:space="preserve">Spatial variables shaded grey as this section of the spreadsheet has not been updated in a while. </t>
+  </si>
+  <si>
+    <t>Level of availability</t>
+  </si>
+  <si>
+    <t>MSOA, LSOA, OA</t>
+  </si>
+  <si>
+    <t>MSOA, LSOA, LA</t>
+  </si>
+  <si>
+    <t>MSOA, LSOA</t>
+  </si>
+  <si>
+    <t>MSOA</t>
   </si>
 </sst>
 </file>
@@ -3695,35 +3710,34 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3733,23 +3747,23 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3828,7 +3842,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4116,7 +4130,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4124,54 +4138,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7970A03-BB7D-4E2A-9D2B-B2C8D50FE960}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="7" customWidth="1"/>
-    <col min="2" max="3" width="22.19921875" style="8"/>
-    <col min="4" max="4" width="22.19921875" style="7"/>
-    <col min="5" max="6" width="22.19921875" style="8"/>
-    <col min="7" max="7" width="22.19921875" style="7"/>
-    <col min="8" max="8" width="63" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="22.19921875" style="19"/>
+    <col min="2" max="3" width="22.1640625" style="8"/>
+    <col min="4" max="4" width="22.1640625" style="7"/>
+    <col min="5" max="6" width="22.1640625" style="8"/>
+    <col min="7" max="7" width="22.1640625" style="7"/>
+    <col min="8" max="8" width="22.1640625" style="8"/>
+    <col min="9" max="9" width="63" style="18" customWidth="1"/>
+    <col min="10" max="16384" width="22.1640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="18" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="17" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>681</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>832</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>833</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>834</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>919</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>920</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>921</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>922</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>369</v>
       </c>
@@ -4193,14 +4211,17 @@
       <c r="G2" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>937</v>
       </c>
-      <c r="I2" s="9">
+      <c r="J2" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>455</v>
       </c>
@@ -4222,11 +4243,14 @@
       <c r="G3" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="H3" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>448</v>
       </c>
@@ -4248,14 +4272,17 @@
       <c r="G4" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>923</v>
       </c>
-      <c r="I4" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="J4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>449</v>
       </c>
@@ -4277,14 +4304,17 @@
       <c r="G5" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>924</v>
       </c>
-      <c r="I5" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>453</v>
       </c>
@@ -4306,11 +4336,14 @@
       <c r="G6" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="I6" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="H6" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>424</v>
       </c>
@@ -4332,14 +4365,17 @@
       <c r="G7" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>936</v>
       </c>
-      <c r="I7" s="9">
+      <c r="J7" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>426</v>
       </c>
@@ -4361,11 +4397,14 @@
       <c r="G8" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="I8" s="9">
+      <c r="H8" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="J8" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>428</v>
       </c>
@@ -4387,11 +4426,14 @@
       <c r="G9" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="I9" s="9">
+      <c r="H9" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="J9" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>430</v>
       </c>
@@ -4413,14 +4455,17 @@
       <c r="G10" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I10" s="19" t="s">
         <v>925</v>
       </c>
-      <c r="I10" s="9">
+      <c r="J10" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -4442,14 +4487,17 @@
       <c r="G11" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>916</v>
       </c>
-      <c r="I11" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="9" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="9" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>422</v>
       </c>
@@ -4471,14 +4519,17 @@
       <c r="G12" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>926</v>
       </c>
-      <c r="I12" s="9">
+      <c r="J12" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>367</v>
       </c>
@@ -4500,14 +4551,17 @@
       <c r="G13" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>898</v>
       </c>
-      <c r="I13" s="9">
+      <c r="J13" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="9" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="9" customFormat="1" ht="170" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>377</v>
       </c>
@@ -4529,14 +4583,17 @@
       <c r="G14" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>927</v>
       </c>
-      <c r="I14" s="9">
+      <c r="J14" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="10" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="10" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>735</v>
       </c>
@@ -4558,14 +4615,17 @@
       <c r="G15" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="6" t="s">
+        <v>946</v>
+      </c>
+      <c r="I15" s="20" t="s">
         <v>928</v>
       </c>
-      <c r="I15" s="10">
+      <c r="J15" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="9" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="9" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>363</v>
       </c>
@@ -4587,14 +4647,17 @@
       <c r="G16" s="4" t="s">
         <v>658</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="I16" s="19" t="s">
         <v>929</v>
       </c>
-      <c r="I16" s="9">
+      <c r="J16" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>689</v>
       </c>
@@ -4616,14 +4679,17 @@
       <c r="G17" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I17" s="19" t="s">
         <v>899</v>
       </c>
-      <c r="I17" s="9">
+      <c r="J17" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>690</v>
       </c>
@@ -4645,11 +4711,14 @@
       <c r="G18" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="I18" s="9">
+      <c r="H18" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J18" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>361</v>
       </c>
@@ -4671,116 +4740,131 @@
       <c r="G19" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I19" s="19" t="s">
         <v>930</v>
       </c>
-      <c r="I19" s="9">
+      <c r="J19" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:10" s="13" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12" t="s">
         <v>829</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>823</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>853</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="12" t="s">
         <v>784</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I20" s="13" t="s">
         <v>938</v>
       </c>
-      <c r="I20" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="J20" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="13" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12" t="s">
         <v>830</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>823</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>888</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="12" t="s">
         <v>785</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="I21" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="H21" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="13" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12" t="s">
         <v>831</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>823</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>854</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="12" t="s">
         <v>786</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="I22" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="H22" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J22" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="13" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12" t="s">
         <v>758</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>828</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>852</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="12" t="s">
         <v>783</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>670</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I23" s="21" t="s">
         <v>931</v>
       </c>
-      <c r="I23" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" ht="296.39999999999998" x14ac:dyDescent="0.3">
+      <c r="J23" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="9" customFormat="1" ht="323" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>683</v>
       </c>
@@ -4802,14 +4886,17 @@
       <c r="G24" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I24" s="9" t="s">
         <v>939</v>
       </c>
-      <c r="I24" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="9" customFormat="1" ht="218.4" x14ac:dyDescent="0.3">
+      <c r="J24" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="9" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>684</v>
       </c>
@@ -4831,14 +4918,17 @@
       <c r="G25" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I25" s="9" t="s">
         <v>918</v>
       </c>
-      <c r="I25" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="9" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="J25" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>685</v>
       </c>
@@ -4860,11 +4950,14 @@
       <c r="G26" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="I26" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="9" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="H26" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J26" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="9" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>686</v>
       </c>
@@ -4886,14 +4979,17 @@
       <c r="G27" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I27" s="19" t="s">
         <v>808</v>
       </c>
-      <c r="I27" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="9" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="J27" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>687</v>
       </c>
@@ -4915,14 +5011,17 @@
       <c r="G28" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I28" s="19" t="s">
         <v>807</v>
       </c>
-      <c r="I28" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="J28" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="9" customFormat="1" ht="187" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>793</v>
       </c>
@@ -4944,14 +5043,17 @@
       <c r="G29" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I29" s="9" t="s">
         <v>932</v>
       </c>
-      <c r="I29" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="J29" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="9" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>365</v>
       </c>
@@ -4973,14 +5075,17 @@
       <c r="G30" s="4" t="s">
         <v>798</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I30" s="19" t="s">
         <v>933</v>
       </c>
-      <c r="I30" s="9">
+      <c r="J30" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>451</v>
       </c>
@@ -5002,11 +5107,14 @@
       <c r="G31" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="I31" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="9" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="H31" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="9" customFormat="1" ht="170" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>84</v>
       </c>
@@ -5028,14 +5136,17 @@
       <c r="G32" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I32" s="9" t="s">
         <v>934</v>
       </c>
-      <c r="I32" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="J32" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
@@ -5057,14 +5168,17 @@
       <c r="G33" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I33" s="9" t="s">
         <v>935</v>
       </c>
-      <c r="I33" s="9">
+      <c r="J33" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
@@ -5086,11 +5200,14 @@
       <c r="G34" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="I34" s="9">
+      <c r="H34" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J34" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>726</v>
       </c>
@@ -5112,11 +5229,14 @@
       <c r="G35" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="I35" s="9">
+      <c r="H35" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J35" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
@@ -5138,11 +5258,14 @@
       <c r="G36" s="4" t="s">
         <v>917</v>
       </c>
-      <c r="I36" s="9">
+      <c r="H36" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J36" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>3</v>
       </c>
@@ -5164,11 +5287,14 @@
       <c r="G37" s="4" t="s">
         <v>917</v>
       </c>
-      <c r="I37" s="9">
+      <c r="H37" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J37" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -5190,11 +5316,14 @@
       <c r="G38" s="4" t="s">
         <v>917</v>
       </c>
-      <c r="I38" s="9">
+      <c r="H38" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J38" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>3</v>
       </c>
@@ -5212,14 +5341,17 @@
       <c r="G39" s="4" t="s">
         <v>917</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H39" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I39" s="9" t="s">
         <v>806</v>
       </c>
-      <c r="I39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="9" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>444</v>
       </c>
@@ -5241,14 +5373,17 @@
       <c r="G40" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>940</v>
       </c>
-      <c r="I40" s="9">
+      <c r="J40" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>446</v>
       </c>
@@ -5270,365 +5405,384 @@
       <c r="G41" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="I41" s="9">
+      <c r="H41" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J41" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="25" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
+    <row r="42" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" s="22" t="s">
         <v>691</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24" t="s">
+      <c r="B42" s="23"/>
+      <c r="C42" s="23" t="s">
         <v>672</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
+      <c r="E42" s="23"/>
+      <c r="F42" s="23" t="s">
         <v>676</v>
       </c>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="23"/>
+      <c r="I42" s="24" t="s">
         <v>941</v>
       </c>
-      <c r="I42" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="25" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="23" t="s">
+      <c r="J42" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="22" t="s">
         <v>692</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24" t="s">
+      <c r="B43" s="23"/>
+      <c r="C43" s="23" t="s">
         <v>673</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="23"/>
+      <c r="F43" s="23" t="s">
         <v>677</v>
       </c>
-      <c r="G43" s="23" t="s">
+      <c r="G43" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="I43" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="25" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="23" t="s">
+      <c r="H43" s="23"/>
+      <c r="J43" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24" t="s">
+      <c r="B44" s="23"/>
+      <c r="C44" s="23" t="s">
         <v>674</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="23"/>
+      <c r="F44" s="23" t="s">
         <v>678</v>
       </c>
-      <c r="G44" s="23" t="s">
+      <c r="G44" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="I44" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="23" t="s">
+      <c r="H44" s="23"/>
+      <c r="J44" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A45" s="22" t="s">
         <v>694</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24" t="s">
+      <c r="B45" s="23"/>
+      <c r="C45" s="23" t="s">
         <v>675</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24" t="s">
+      <c r="E45" s="23"/>
+      <c r="F45" s="23" t="s">
         <v>679</v>
       </c>
-      <c r="G45" s="23" t="s">
+      <c r="G45" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="I45" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="25" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+      <c r="H45" s="23"/>
+      <c r="J45" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="22" t="s">
         <v>697</v>
       </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24" t="s">
+      <c r="B46" s="23"/>
+      <c r="C46" s="23" t="s">
         <v>695</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="D46" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24" t="s">
+      <c r="E46" s="23"/>
+      <c r="F46" s="23" t="s">
         <v>696</v>
       </c>
-      <c r="G46" s="23" t="s">
+      <c r="G46" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="I46" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="23" t="s">
+      <c r="H46" s="23"/>
+      <c r="J46" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="22" t="s">
         <v>720</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24" t="s">
+      <c r="B47" s="23"/>
+      <c r="C47" s="23" t="s">
         <v>698</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24" t="s">
+      <c r="E47" s="23"/>
+      <c r="F47" s="23" t="s">
         <v>708</v>
       </c>
-      <c r="G47" s="23" t="s">
+      <c r="G47" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I47" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="23" t="s">
+      <c r="H47" s="23"/>
+      <c r="J47" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="22" t="s">
         <v>716</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24" t="s">
+      <c r="B48" s="23"/>
+      <c r="C48" s="23" t="s">
         <v>699</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="D48" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24" t="s">
+      <c r="E48" s="23"/>
+      <c r="F48" s="23" t="s">
         <v>709</v>
       </c>
-      <c r="G48" s="23" t="s">
+      <c r="G48" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I48" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="23" t="s">
+      <c r="H48" s="23"/>
+      <c r="J48" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A49" s="22" t="s">
         <v>717</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24" t="s">
+      <c r="B49" s="23"/>
+      <c r="C49" s="23" t="s">
         <v>700</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24" t="s">
+      <c r="E49" s="23"/>
+      <c r="F49" s="23" t="s">
         <v>727</v>
       </c>
-      <c r="G49" s="23" t="s">
+      <c r="G49" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I49" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="25" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="23" t="s">
+      <c r="H49" s="23"/>
+      <c r="J49" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="24" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A50" s="22" t="s">
         <v>718</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24" t="s">
+      <c r="B50" s="23"/>
+      <c r="C50" s="23" t="s">
         <v>701</v>
       </c>
-      <c r="D50" s="23" t="s">
+      <c r="D50" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24" t="s">
+      <c r="E50" s="23"/>
+      <c r="F50" s="23" t="s">
         <v>710</v>
       </c>
-      <c r="G50" s="23" t="s">
+      <c r="G50" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="H50" s="25" t="s">
+      <c r="H50" s="23"/>
+      <c r="I50" s="24" t="s">
         <v>766</v>
       </c>
-      <c r="I50" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="25" customFormat="1" ht="78" x14ac:dyDescent="0.3">
-      <c r="A51" s="23" t="s">
+      <c r="J50" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="24" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A51" s="22" t="s">
         <v>719</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24" t="s">
+      <c r="B51" s="23"/>
+      <c r="C51" s="23" t="s">
         <v>702</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="D51" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24" t="s">
+      <c r="E51" s="23"/>
+      <c r="F51" s="23" t="s">
         <v>711</v>
       </c>
-      <c r="G51" s="23" t="s">
+      <c r="G51" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I51" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="23" t="s">
+      <c r="H51" s="23"/>
+      <c r="J51" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A52" s="22" t="s">
         <v>721</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24" t="s">
+      <c r="B52" s="23"/>
+      <c r="C52" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24" t="s">
+      <c r="E52" s="23"/>
+      <c r="F52" s="23" t="s">
         <v>712</v>
       </c>
-      <c r="G52" s="23" t="s">
+      <c r="G52" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I52" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="23" t="s">
+      <c r="H52" s="23"/>
+      <c r="J52" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" s="22" t="s">
         <v>722</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24" t="s">
+      <c r="B53" s="23"/>
+      <c r="C53" s="23" t="s">
         <v>703</v>
       </c>
-      <c r="D53" s="23" t="s">
+      <c r="D53" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24" t="s">
+      <c r="E53" s="23"/>
+      <c r="F53" s="23" t="s">
         <v>713</v>
       </c>
-      <c r="G53" s="23" t="s">
+      <c r="G53" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I53" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="23" t="s">
+      <c r="H53" s="23"/>
+      <c r="J53" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A54" s="22" t="s">
         <v>724</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24" t="s">
+      <c r="B54" s="23"/>
+      <c r="C54" s="23" t="s">
         <v>705</v>
       </c>
-      <c r="D54" s="23" t="s">
+      <c r="D54" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24" t="s">
+      <c r="E54" s="23"/>
+      <c r="F54" s="23" t="s">
         <v>728</v>
       </c>
-      <c r="G54" s="23" t="s">
+      <c r="G54" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I54" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="25" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="23" t="s">
+      <c r="H54" s="23"/>
+      <c r="J54" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A55" s="22" t="s">
         <v>725</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24" t="s">
+      <c r="B55" s="23"/>
+      <c r="C55" s="23" t="s">
         <v>706</v>
       </c>
-      <c r="D55" s="23" t="s">
+      <c r="D55" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24" t="s">
+      <c r="E55" s="23"/>
+      <c r="F55" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="G55" s="23" t="s">
+      <c r="G55" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I55" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="25" customFormat="1" ht="78" x14ac:dyDescent="0.3">
-      <c r="A56" s="23" t="s">
+      <c r="H55" s="23"/>
+      <c r="J55" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="24" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A56" s="22" t="s">
         <v>723</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24" t="s">
+      <c r="B56" s="23"/>
+      <c r="C56" s="23" t="s">
         <v>707</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24" t="s">
+      <c r="E56" s="23"/>
+      <c r="F56" s="23" t="s">
         <v>715</v>
       </c>
-      <c r="G56" s="23" t="s">
+      <c r="G56" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I56" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="25" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="23" t="s">
+      <c r="H56" s="23"/>
+      <c r="J56" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A57" s="22" t="s">
         <v>729</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24" t="s">
+      <c r="B57" s="23"/>
+      <c r="C57" s="23" t="s">
         <v>730</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="D57" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24" t="s">
+      <c r="E57" s="23"/>
+      <c r="F57" s="23" t="s">
         <v>731</v>
       </c>
-      <c r="G57" s="23" t="s">
+      <c r="G57" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="I57" s="25">
+      <c r="H57" s="23"/>
+      <c r="J57" s="24">
         <v>2</v>
       </c>
     </row>
@@ -5648,14 +5802,14 @@
       <selection pane="bottomLeft" activeCell="B336" sqref="B336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5678,7 +5832,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -5695,7 +5849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>353</v>
       </c>
@@ -5712,7 +5866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>355</v>
       </c>
@@ -5729,7 +5883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>357</v>
       </c>
@@ -5746,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>359</v>
       </c>
@@ -5766,7 +5920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -5786,7 +5940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>363</v>
       </c>
@@ -5806,7 +5960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>365</v>
       </c>
@@ -5826,7 +5980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>367</v>
       </c>
@@ -5846,7 +6000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>369</v>
       </c>
@@ -5866,7 +6020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>371</v>
       </c>
@@ -5886,7 +6040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>373</v>
       </c>
@@ -5906,7 +6060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>375</v>
       </c>
@@ -5923,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>377</v>
       </c>
@@ -5943,7 +6097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>383</v>
       </c>
@@ -5960,7 +6114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>392</v>
       </c>
@@ -5977,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>432</v>
       </c>
@@ -5997,7 +6151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>434</v>
       </c>
@@ -6017,7 +6171,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>436</v>
       </c>
@@ -6037,7 +6191,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>438</v>
       </c>
@@ -6057,7 +6211,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>440</v>
       </c>
@@ -6077,7 +6231,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>442</v>
       </c>
@@ -6097,7 +6251,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>444</v>
       </c>
@@ -6117,7 +6271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>446</v>
       </c>
@@ -6137,7 +6291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>448</v>
       </c>
@@ -6160,7 +6314,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>449</v>
       </c>
@@ -6183,7 +6337,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>451</v>
       </c>
@@ -6206,7 +6360,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>453</v>
       </c>
@@ -6229,7 +6383,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>455</v>
       </c>
@@ -6252,7 +6406,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>528</v>
       </c>
@@ -6269,7 +6423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>529</v>
       </c>
@@ -6286,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>422</v>
       </c>
@@ -6306,7 +6460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>424</v>
       </c>
@@ -6326,7 +6480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>426</v>
       </c>
@@ -6346,7 +6500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>428</v>
       </c>
@@ -6366,7 +6520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>430</v>
       </c>
@@ -6386,7 +6540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -6403,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -6423,7 +6577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -6443,7 +6597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -6463,7 +6617,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -6483,7 +6637,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -6503,7 +6657,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -6523,7 +6677,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -6543,7 +6697,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -6563,7 +6717,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -6583,7 +6737,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -6603,7 +6757,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -6623,7 +6777,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -6643,7 +6797,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -6660,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -6683,7 +6837,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>406</v>
       </c>
@@ -6700,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -6717,7 +6871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>410</v>
       </c>
@@ -6734,7 +6888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>412</v>
       </c>
@@ -6751,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>414</v>
       </c>
@@ -6768,7 +6922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>416</v>
       </c>
@@ -6785,7 +6939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>418</v>
       </c>
@@ -6802,7 +6956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>420</v>
       </c>
@@ -6819,7 +6973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>509</v>
       </c>
@@ -6836,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>520</v>
       </c>
@@ -6853,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>521</v>
       </c>
@@ -6870,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -6887,7 +7041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>523</v>
       </c>
@@ -6904,7 +7058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>530</v>
       </c>
@@ -6921,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>531</v>
       </c>
@@ -6938,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>532</v>
       </c>
@@ -6955,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>231</v>
       </c>
@@ -6972,7 +7126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>232</v>
       </c>
@@ -6989,7 +7143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>233</v>
       </c>
@@ -7006,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>234</v>
       </c>
@@ -7023,7 +7177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>235</v>
       </c>
@@ -7040,7 +7194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>236</v>
       </c>
@@ -7057,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>237</v>
       </c>
@@ -7074,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>238</v>
       </c>
@@ -7091,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>239</v>
       </c>
@@ -7108,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>240</v>
       </c>
@@ -7125,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>241</v>
       </c>
@@ -7142,7 +7296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>242</v>
       </c>
@@ -7159,7 +7313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>243</v>
       </c>
@@ -7176,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>69</v>
       </c>
@@ -7193,7 +7347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>73</v>
       </c>
@@ -7210,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -7227,7 +7381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>21</v>
       </c>
@@ -7250,7 +7404,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -7273,7 +7427,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -7290,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>398</v>
       </c>
@@ -7313,7 +7467,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>399</v>
       </c>
@@ -7336,7 +7490,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>400</v>
       </c>
@@ -7359,7 +7513,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>401</v>
       </c>
@@ -7376,7 +7530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -7395,11 +7549,11 @@
       <c r="F92">
         <v>2</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G92" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>56</v>
       </c>
@@ -7422,7 +7576,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>57</v>
       </c>
@@ -7445,7 +7599,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -7468,7 +7622,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -7491,7 +7645,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -7508,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>63</v>
       </c>
@@ -7531,7 +7685,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>64</v>
       </c>
@@ -7554,7 +7708,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>65</v>
       </c>
@@ -7577,7 +7731,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>66</v>
       </c>
@@ -7600,7 +7754,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>67</v>
       </c>
@@ -7623,7 +7777,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>68</v>
       </c>
@@ -7640,7 +7794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>75</v>
       </c>
@@ -7663,7 +7817,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>86</v>
       </c>
@@ -7686,7 +7840,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>87</v>
       </c>
@@ -7703,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>27</v>
       </c>
@@ -7720,7 +7874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -7737,7 +7891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>29</v>
       </c>
@@ -7757,7 +7911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -7777,7 +7931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>32</v>
       </c>
@@ -7797,7 +7951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -7814,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>34</v>
       </c>
@@ -7831,7 +7985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -7851,7 +8005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -7868,7 +8022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>38</v>
       </c>
@@ -7888,7 +8042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>45</v>
       </c>
@@ -7905,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>46</v>
       </c>
@@ -7922,7 +8076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>47</v>
       </c>
@@ -7939,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -7956,7 +8110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>49</v>
       </c>
@@ -7973,7 +8127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>50</v>
       </c>
@@ -7990,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -8013,7 +8167,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>90</v>
       </c>
@@ -8036,7 +8190,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>92</v>
       </c>
@@ -8059,7 +8213,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>94</v>
       </c>
@@ -8082,7 +8236,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>96</v>
       </c>
@@ -8105,7 +8259,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>98</v>
       </c>
@@ -8128,7 +8282,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>100</v>
       </c>
@@ -8151,7 +8305,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>102</v>
       </c>
@@ -8174,7 +8328,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>104</v>
       </c>
@@ -8197,7 +8351,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>106</v>
       </c>
@@ -8220,7 +8374,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>108</v>
       </c>
@@ -8243,7 +8397,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>110</v>
       </c>
@@ -8266,7 +8420,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>112</v>
       </c>
@@ -8289,7 +8443,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>114</v>
       </c>
@@ -8312,7 +8466,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>116</v>
       </c>
@@ -8335,7 +8489,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>118</v>
       </c>
@@ -8358,7 +8512,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>120</v>
       </c>
@@ -8381,7 +8535,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>122</v>
       </c>
@@ -8404,7 +8558,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>124</v>
       </c>
@@ -8427,7 +8581,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>126</v>
       </c>
@@ -8450,7 +8604,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>128</v>
       </c>
@@ -8473,7 +8627,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>130</v>
       </c>
@@ -8496,7 +8650,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>132</v>
       </c>
@@ -8519,7 +8673,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>134</v>
       </c>
@@ -8542,7 +8696,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>136</v>
       </c>
@@ -8565,7 +8719,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>138</v>
       </c>
@@ -8588,7 +8742,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>140</v>
       </c>
@@ -8611,7 +8765,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>142</v>
       </c>
@@ -8634,7 +8788,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>144</v>
       </c>
@@ -8657,7 +8811,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>146</v>
       </c>
@@ -8680,7 +8834,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>148</v>
       </c>
@@ -8703,7 +8857,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>150</v>
       </c>
@@ -8726,7 +8880,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -8749,7 +8903,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -8772,7 +8926,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -8795,7 +8949,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>158</v>
       </c>
@@ -8818,7 +8972,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -8841,7 +8995,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>162</v>
       </c>
@@ -8864,7 +9018,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>164</v>
       </c>
@@ -8887,7 +9041,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>166</v>
       </c>
@@ -8910,7 +9064,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>168</v>
       </c>
@@ -8933,7 +9087,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -8956,7 +9110,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -8979,7 +9133,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>174</v>
       </c>
@@ -9002,7 +9156,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>176</v>
       </c>
@@ -9025,7 +9179,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>178</v>
       </c>
@@ -9048,7 +9202,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>180</v>
       </c>
@@ -9071,7 +9225,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>182</v>
       </c>
@@ -9094,7 +9248,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>184</v>
       </c>
@@ -9117,7 +9271,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>186</v>
       </c>
@@ -9140,7 +9294,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>188</v>
       </c>
@@ -9163,7 +9317,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -9186,7 +9340,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>192</v>
       </c>
@@ -9209,7 +9363,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>194</v>
       </c>
@@ -9232,7 +9386,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>200</v>
       </c>
@@ -9255,7 +9409,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>202</v>
       </c>
@@ -9278,7 +9432,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>204</v>
       </c>
@@ -9301,7 +9455,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>206</v>
       </c>
@@ -9324,7 +9478,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>208</v>
       </c>
@@ -9347,7 +9501,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>210</v>
       </c>
@@ -9370,7 +9524,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>212</v>
       </c>
@@ -9393,7 +9547,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>214</v>
       </c>
@@ -9416,7 +9570,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>216</v>
       </c>
@@ -9439,7 +9593,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>218</v>
       </c>
@@ -9456,7 +9610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>270</v>
       </c>
@@ -9479,7 +9633,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>290</v>
       </c>
@@ -9502,7 +9656,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>310</v>
       </c>
@@ -9525,7 +9679,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>330</v>
       </c>
@@ -9548,7 +9702,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>512</v>
       </c>
@@ -9571,7 +9725,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>278</v>
       </c>
@@ -9594,7 +9748,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>298</v>
       </c>
@@ -9617,7 +9771,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>318</v>
       </c>
@@ -9640,7 +9794,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>338</v>
       </c>
@@ -9663,7 +9817,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>282</v>
       </c>
@@ -9686,7 +9840,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>302</v>
       </c>
@@ -9709,7 +9863,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>322</v>
       </c>
@@ -9732,7 +9886,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>342</v>
       </c>
@@ -9755,7 +9909,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>518</v>
       </c>
@@ -9778,7 +9932,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>286</v>
       </c>
@@ -9801,7 +9955,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>306</v>
       </c>
@@ -9824,7 +9978,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>326</v>
       </c>
@@ -9847,7 +10001,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>346</v>
       </c>
@@ -9870,7 +10024,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>510</v>
       </c>
@@ -9893,7 +10047,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>274</v>
       </c>
@@ -9916,7 +10070,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>294</v>
       </c>
@@ -9939,7 +10093,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>314</v>
       </c>
@@ -9962,7 +10116,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>334</v>
       </c>
@@ -9985,7 +10139,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>513</v>
       </c>
@@ -10008,7 +10162,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>272</v>
       </c>
@@ -10031,7 +10185,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>292</v>
       </c>
@@ -10054,7 +10208,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>312</v>
       </c>
@@ -10077,7 +10231,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>332</v>
       </c>
@@ -10100,7 +10254,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>516</v>
       </c>
@@ -10123,7 +10277,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>280</v>
       </c>
@@ -10146,7 +10300,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>300</v>
       </c>
@@ -10169,7 +10323,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>320</v>
       </c>
@@ -10192,7 +10346,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>340</v>
       </c>
@@ -10215,7 +10369,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>515</v>
       </c>
@@ -10238,7 +10392,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>284</v>
       </c>
@@ -10261,7 +10415,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>304</v>
       </c>
@@ -10284,7 +10438,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>324</v>
       </c>
@@ -10307,7 +10461,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>344</v>
       </c>
@@ -10330,7 +10484,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>519</v>
       </c>
@@ -10353,7 +10507,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>288</v>
       </c>
@@ -10376,7 +10530,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>308</v>
       </c>
@@ -10399,7 +10553,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>328</v>
       </c>
@@ -10422,7 +10576,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>348</v>
       </c>
@@ -10445,7 +10599,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>514</v>
       </c>
@@ -10468,7 +10622,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>276</v>
       </c>
@@ -10491,7 +10645,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>296</v>
       </c>
@@ -10514,7 +10668,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>316</v>
       </c>
@@ -10537,7 +10691,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>336</v>
       </c>
@@ -10560,7 +10714,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>517</v>
       </c>
@@ -10583,7 +10737,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>652</v>
       </c>
@@ -10602,9 +10756,8 @@
       <c r="F236">
         <v>3</v>
       </c>
-      <c r="G236" s="11"/>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>653</v>
       </c>
@@ -10623,9 +10776,8 @@
       <c r="F237">
         <v>3</v>
       </c>
-      <c r="G237" s="11"/>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>654</v>
       </c>
@@ -10644,9 +10796,8 @@
       <c r="F238">
         <v>3</v>
       </c>
-      <c r="G238" s="11"/>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>655</v>
       </c>
@@ -10665,9 +10816,8 @@
       <c r="F239">
         <v>3</v>
       </c>
-      <c r="G239" s="11"/>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>656</v>
       </c>
@@ -10686,9 +10836,8 @@
       <c r="F240">
         <v>3</v>
       </c>
-      <c r="G240" s="11"/>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>350</v>
       </c>
@@ -10705,7 +10854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>351</v>
       </c>
@@ -10722,7 +10871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>352</v>
       </c>
@@ -10739,7 +10888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>31</v>
       </c>
@@ -10753,7 +10902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>37</v>
       </c>
@@ -10767,7 +10916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>39</v>
       </c>
@@ -10781,7 +10930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>41</v>
       </c>
@@ -10795,7 +10944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>42</v>
       </c>
@@ -10809,7 +10958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>43</v>
       </c>
@@ -10823,7 +10972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>44</v>
       </c>
@@ -10837,7 +10986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>51</v>
       </c>
@@ -10851,7 +11000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>52</v>
       </c>
@@ -10865,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>53</v>
       </c>
@@ -10879,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>54</v>
       </c>
@@ -10895,11 +11044,11 @@
       <c r="F254">
         <v>2</v>
       </c>
-      <c r="G254" s="11" t="s">
+      <c r="G254" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>62</v>
       </c>
@@ -10915,11 +11064,11 @@
       <c r="F255">
         <v>2</v>
       </c>
-      <c r="G255" s="11" t="s">
+      <c r="G255" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>77</v>
       </c>
@@ -10933,7 +11082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>79</v>
       </c>
@@ -10947,7 +11096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>85</v>
       </c>
@@ -10961,7 +11110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>196</v>
       </c>
@@ -10975,7 +11124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>197</v>
       </c>
@@ -10989,7 +11138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>198</v>
       </c>
@@ -11003,7 +11152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>199</v>
       </c>
@@ -11017,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>219</v>
       </c>
@@ -11031,7 +11180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>221</v>
       </c>
@@ -11045,7 +11194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>223</v>
       </c>
@@ -11059,7 +11208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>225</v>
       </c>
@@ -11073,7 +11222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>227</v>
       </c>
@@ -11087,7 +11236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>229</v>
       </c>
@@ -11101,7 +11250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>244</v>
       </c>
@@ -11115,7 +11264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>246</v>
       </c>
@@ -11129,7 +11278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>248</v>
       </c>
@@ -11143,7 +11292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>250</v>
       </c>
@@ -11157,7 +11306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>252</v>
       </c>
@@ -11171,7 +11320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>254</v>
       </c>
@@ -11185,7 +11334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>256</v>
       </c>
@@ -11199,7 +11348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>258</v>
       </c>
@@ -11213,7 +11362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>260</v>
       </c>
@@ -11227,7 +11376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>262</v>
       </c>
@@ -11241,7 +11390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>264</v>
       </c>
@@ -11255,7 +11404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>266</v>
       </c>
@@ -11269,7 +11418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>268</v>
       </c>
@@ -11283,7 +11432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>379</v>
       </c>
@@ -11303,7 +11452,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>381</v>
       </c>
@@ -11317,7 +11466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>385</v>
       </c>
@@ -11331,7 +11480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>387</v>
       </c>
@@ -11345,7 +11494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>389</v>
       </c>
@@ -11359,7 +11508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>390</v>
       </c>
@@ -11373,7 +11522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>394</v>
       </c>
@@ -11387,7 +11536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>396</v>
       </c>
@@ -11401,7 +11550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>402</v>
       </c>
@@ -11415,7 +11564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>404</v>
       </c>
@@ -11429,7 +11578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>457</v>
       </c>
@@ -11443,7 +11592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>459</v>
       </c>
@@ -11457,7 +11606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>461</v>
       </c>
@@ -11471,7 +11620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>463</v>
       </c>
@@ -11485,7 +11634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>465</v>
       </c>
@@ -11499,7 +11648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>467</v>
       </c>
@@ -11513,7 +11662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>469</v>
       </c>
@@ -11527,7 +11676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>471</v>
       </c>
@@ -11541,7 +11690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>473</v>
       </c>
@@ -11555,7 +11704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>475</v>
       </c>
@@ -11569,7 +11718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>477</v>
       </c>
@@ -11583,7 +11732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>478</v>
       </c>
@@ -11597,7 +11746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>479</v>
       </c>
@@ -11611,7 +11760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>480</v>
       </c>
@@ -11625,7 +11774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>481</v>
       </c>
@@ -11639,7 +11788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>482</v>
       </c>
@@ -11653,7 +11802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>483</v>
       </c>
@@ -11667,7 +11816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>484</v>
       </c>
@@ -11681,7 +11830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>485</v>
       </c>
@@ -11695,7 +11844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>487</v>
       </c>
@@ -11709,7 +11858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>489</v>
       </c>
@@ -11723,7 +11872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>491</v>
       </c>
@@ -11737,7 +11886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>493</v>
       </c>
@@ -11751,7 +11900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>495</v>
       </c>
@@ -11765,7 +11914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>497</v>
       </c>
@@ -11779,7 +11928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>499</v>
       </c>
@@ -11793,7 +11942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>501</v>
       </c>
@@ -11807,7 +11956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>503</v>
       </c>
@@ -11821,7 +11970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>505</v>
       </c>
@@ -11835,7 +11984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>507</v>
       </c>
@@ -11849,7 +11998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>511</v>
       </c>
@@ -11864,7 +12013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>524</v>
       </c>
@@ -11878,7 +12027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>526</v>
       </c>

</xml_diff>